<commit_message>
Get daily reddit data: Tue Jan  2 08:08:35 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_07.xlsx
+++ b/data/2024_01_07.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C441"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2386 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>18wjo6y</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Is it possible to put my nail line/free edge to the top of my fingers so there is less white and more pink?</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18wjo6y/is_it_possible_to_put_my_nail_linefree_edge_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>18wdk6y</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Is it normal for acrylics to break within 24 hours?</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdwwpketpx9c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>18wiuow</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>How often do you go to a salon and do you prefer desigb over durability?</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18wiuow/how_often_do_you_go_to_a_salon_and_do_you_prefer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>18wiknx</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>My first attempt at builder gel!</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wiknx</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>18wij6u</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Pretty pink practice! I’m still new to this but I just love how this turned out!</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wij6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>18wic12</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>i’m obsessed 🌌</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rwrcr2oxwy9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>18whp69</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>First set of gel nails! Thoughts?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18whp69</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>18wh4ao</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Best French Tip Press Ons?</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18wh4ao/best_french_tip_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>18w7ja2</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>I really need help</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18w7ja2/i_really_need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>18wfhgw</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>I can’t help myself with these!</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dimqqli26y9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>18wego0</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>My New Years nails!</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqsvs1j9xx9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>18weeyp</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Good strengthening polish?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18weeyp/good_strengthening_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>18we5z0</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Holiday nails ✨️</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0ixqsrtux9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>18wdy8v</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Took 4 hours but well worth it💚🖤</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wdy8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>18wcvmz</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Has anyone here bought anything from samnailsupply dot com? Is it legitimate?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18wcvmz/has_anyone_here_bought_anything_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>18wcsqg</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>First time nails</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y966wzxdjx9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>18wcrve</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Frenchies</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iectm055jx9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>18wckqo</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Charms</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wckqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>18wcdtd</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>My nail tech gets me…</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ma2fqs8wfx9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>18wccac</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>seche vite smell</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18wccac/seche_vite_smell/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>18wbr2a</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>happy new year everyone 🌟🎊</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wbr2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>18wbo55</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>My natural babies🥰</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wbo55</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>18wb9mw</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>What’s your favorite professional builder gel in a tub and where do you get it?</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18wb9mw/whats_your_favorite_professional_builder_gel_in_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>18wb345</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>happy new year! :)</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkjgvzzl5x9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>18wb1ez</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Got a nee magnetic polish. I'm in absolute LOVE.</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmr929j95x9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>18waxkz</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>I love this colour!!</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/799uwq4f4x9c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>18wammn</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>New Year, so I picked up my brush for the first time in a year. All left hand work. Really proud.</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wammn</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>18wacc3</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Why are there 13 yr olds saying they are nail techs?</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18wacc3/why_are_there_13_yr_olds_saying_they_are_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>18wabp1</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Happy new year 🎄💝</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wabp1</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>18w9x5j</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>How much would you pay?</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w9x5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>18w9wks</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Happy new year! Hand painted car eye art deco nails by me 🥂✨</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w9wks</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>18w9v8u</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Is this normal grow out for a manicure less than 2 weeks old?</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fip6xui6ww9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>18w8ufh</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Valentines Day is coming! Glitter syrup nails with tiny purple hearts.</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w8ufh</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>18w8fr4</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>How much would you pay for these?</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w8fr4</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>18w83wa</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>(Late) Christmas nails</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w83wa</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>18w7t01</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Almond Baby Boomer construction took 6 HOURS, and maintannce took 5 hours. Is my nail shape the problem. Sorry for the colour, I took this picture when I just dyed my hair red and the colour just wouldn’t leave my nails 🥲</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y91ol83lgw9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>18w73g9</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>this mani gives sexi 🤫🌶️</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c7p4scacbw9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>18w720s</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>My boyfriend helped me do my nails (:</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7q9qgf2bw9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>18w6eo1</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Fresh gel and polish featuring my forever messy cuticles 😌</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okovg3x66w9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>18w4usu</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Is it okay to cut your nails twice a week?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18w4usu/is_it_okay_to_cut_your_nails_twice_a_week/</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>18w4nwz</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Some cute nail art I did. What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w4nwz</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>18w4eab</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Seasons Greetings</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w4eab</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>18w3urc</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Practicing painting nails, need opinions</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nbat1h96nv9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>18w2x7m</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>vertical split occurs whenever nail grows beyond nail bed. help!!</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s93rnn18gv9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>18w2wga</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Winter nails 💅</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfaoh6y1gv9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>18w2k54</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>First time acrylics on myself. How to prevent peeling?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w2k54</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>18w2gut</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Nailzzz 🎉2024</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w2gut</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>18w2cpn</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Made winter press ons</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/73e7zqirbv9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>18w29do</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Any REALLY glittery gel polish i could buy on Amazon?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18w29do/any_really_glittery_gel_polish_i_could_buy_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>18w27fo</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>In love with these</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02fh1wlpav9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>18w0uka</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>How do I stop my nails from doing this BS??</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w0uka</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>18w24xn</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Not sure how I feel. I wanted something subtle, but the shape is what’s throwing me… I think</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qxphdz56av9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>18w21ki</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>My favorite nails so far this year :)</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w21ki</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>18vwo6m</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Question</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18vwo6m</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>18w1zk6</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>This is what $140 nails look like at my workplace :)</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w1zk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>18vnv25</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Need help!</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7bxmkexxq9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>18vjanh</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Just started creating my own press on nails using fluid art technique</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dekp79i9np9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>18vj6yl</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>HoloTaco Dark Rainbow Mani</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18vj6yl</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>18vi84j</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Always see US-based posts, thought to share how it’s like in the UK! £40 for builder gel and to take off my old BIAB set (£30 for in-fills in the future)</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18vi84j</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>18vgmfy</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Why do my nails bubble up sometimes?</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kl8jw0k8zo9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>18vfwq5</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Help me find a nude that works with my skin tone, please.</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18vfwq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>18w1fiq</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Christmas nails worth it?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k17vfd8l4v9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>18w1332</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>New year nails I made on an app.</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w1332</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>18w0z8e</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Last sets of the year! These are all structured gel manicures on my clients natural nails ✨</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w0z8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>18w0rbp</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Question on acrylic nails</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18w0rbp/question_on_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>18w0b24</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Btart Soft Gel Press Ons.</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w0b24</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>18vzdgt</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>first mani of 2024. 💜🥂✨</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0vj2eewnu9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>18vz4qg</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>How to get started on doing your own nails</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18vz4qg/how_to_get_started_on_doing_your_own_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>18vz2in</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>New Year, Same Moody Polish</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mpmzsu9lu9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>18vxs1t</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Last set for 2023</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrmmc9wb9u9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>18vxmix</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Happy New Nails! 💅🎄✨</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18vxmix</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>18vxj55</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Obsessed with this Combo - Bejeweled Nails</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2v4d37u6u9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>18vx6w5</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Where to purchase CND Shellac within the EU as a non-certified nail tach.</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18vx6w5/where_to_purchase_cnd_shellac_within_the_eu_as_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>18vx298</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Winnie the pooh🍯</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0z8sl7sz1u9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>18vwxgu</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>New Years Dip Nails</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6r44oczn0u9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>18vuk84</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Last minute glossy red for NYE!</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25vj5k8r8t9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>18vuizl</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>How to remove glue from applied press on nails</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18vuizl</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>18vu4bz</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>good gel x brands?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18vu4bz/good_gel_x_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>18vttx4</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Tips and Essentials for someone wanting to learn how to do their own nails at home?</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18vttx4/tips_and_essentials_for_someone_wanting_to_learn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>18vt3kc</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time </t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vkkl2jamps9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>18wjfa9</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Storage advice?</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18wjfa9/storage_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>18wgraa</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Does anyone else mix/layer different jelly colors?</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wgraa</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>18wfjvk</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>New year's winter glow</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wfjvk</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>18wfhuu</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Can I use Essie colors with Dazzle Dry top and base coat?</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18wfhuu/can_i_use_essie_colors_with_dazzle_dry_top_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>18weu7z</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Love Purples 💜</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18weu7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>18werw1</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18werw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>18wefxh</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Morgan Taylor Could Have Foiled Me 🪩✨</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rn9ttmn1xx9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>18we7y7</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>First set of 2024</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vj02abavx9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>18wd7uf</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>🥴 New Year's Nails 🥴</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z1xhx9uxmx9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>18wd5ma</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>“Ether Dragon” - A New Years fave!</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wd5ma</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>18wcuwg</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Has anyone here bought anything from samnailsupply dot com? Is it legitimate?</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18wcuwg/has_anyone_here_bought_anything_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>18wcmlk</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Strange the Dreamer</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zgutf4qxhx9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>18wbh0m</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>New Year, Clean Look</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9nql44zm8x9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>18wavua</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Gremlin mode skittle</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8avtjkj14x9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>18w9qcm</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>obsessed with the subtle aqua shift! ILNP Moondust</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w9qcm</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>18w9fae</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Happy new year! Hand painted cat eye art deco nails by me 🥂</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w9fae</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>18w8w7z</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>For science!! “Homemade” Fairy Dust using Take Me To Your Leader</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vkbm6sgrow9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>18w7h09</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Rescue Me</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w7h09</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>18w6oi3</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Definitely not regretting this PPU purchase</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w6oi3</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>18w603o</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>First time trying a sandwich mani</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w603o</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>18w5so3</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>This collection has many beautiful pinks and reds but lacks greens and blues imo. This is one of the few and it's gorgeous! - Kiko Milano Perfect Gel shade #120 hand 💅🏻</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5jej69n1w9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>18w5qps</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>A perfect beginning</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/buxz3nz61w9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>18w5kgh</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>🧲🌈Magnetic Skittle🌈🧲</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w5kgh</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>18w5fvh</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>How my year started vs. how it ended</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w5fvh</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>18w56gc</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Purple for the win!</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w56gc</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>18w54ng</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Warm love, more fun, less worry. Wanted nails to reflect hopes for 2024 ♥️</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w54ng</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>18w4u3s</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>NYE Minimalist</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d15bju5luv9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>18w4rt3</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Does such a polish exist?</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18w4rt3/does_such_a_polish_exist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>18w4k78</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Shiny is mandatory for New Year's, right?</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w4k78</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>18w4iz6</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>What do you think of this silver velvet??</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iy4msn96sv9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>18w3x3z</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Experiment time! Going to be testing the OPI Repair Mode serum on my very damaged thumbnail. Day 1</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://imgur.com/7XfntWu</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>18w3cxt</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>My Dupe Attempt of Phoenix's Cotton Ice Swatch Photos (sans neon glitter)</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w3cxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>18w31v5</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>How to remove fake nails on a gel base?</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18w31v5/how_to_remove_fake_nails_on_a_gel_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>18w2whm</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>I made nail polish out of 🪨</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w2whm</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>18w2ulh</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>My First REAL Attempt at a French Manicure</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w2ulh</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>18w2tob</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Must have ILNP polishes?</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18w2tob/must_have_ilnp_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>18w2qjn</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Nail nail mani pt 2!</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w2qjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>18w2j2o</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>New Year Skittle ✨</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w2j2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>18w1vvv</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>First of 2024</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ff7niec58v9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>18w0oia</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Seeking Advice</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w0oia</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>18w00xd</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Before the LynB website reopens I have a question</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18w00xd/before_the_lynb_website_reopens_i_have_a_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>18vzvo9</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Hello Kitty strawberry shortcake Goldfish cracker feat. my cute nail polish</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5lnzjkn4su9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>18vz3qs</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>New Year, Same Moody Polish</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pvzjjjklu9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>18vyy0r</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Last set for 2023</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6dzu83o5ku9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>18vy9qi</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>New Year Nails!</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18vy9qi</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>18vx9wx</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Felt creative last night, tried Jelly-style nails</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4p2q59jc4u9c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>18vvhkh</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Manifest This</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18vvhkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>18vukyw</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>PPU Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18vukyw/ppu_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>18vukk4</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18vukk4/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>18vthve</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Setting the vibe for 2024 👽</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jb33ug1wus9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>18vsz8s</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>New years nails</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18vsz8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>18wgroq</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Ouch</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cqy3uhuhy9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>18wbzrq</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Nails Rva</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wbzrq</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>18wbr2o</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>New to nail art, making gel press ons, here’s my best ones so far!</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8vxwz8tax9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>18wbf3g</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>New Practice Set</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wbf3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>18wbcty</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>New year, new cute set</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpekra7q7x9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>18wb10t</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Hey Reddit I just did my nails</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4yzvc865x9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>18w9h9y</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Happy new year! Hand painted art deco nails by me 🥂✨</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w9h9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>18w5qnr</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love My Nails </t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rvaes6b81w9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>18vud46</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>MCR nail art (it's not a phase) ☆ hand painted press on nails for the overgrown emo kid</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://youtu.be/Y5NrsTqn-tw?si=U5PAaZNhllJUIFbg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jan  3 08:07:58 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_07.xlsx
+++ b/data/2024_01_07.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C441"/>
+  <dimension ref="A1:C610"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7930,6 +7930,2879 @@
         </is>
       </c>
     </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>18xdw5z</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>🖤</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xdw5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>18xdpxs</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>New year Resolution - to do my own nails.</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9u6s3fwqh6ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>18xboal</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Cracked nail tips</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xboal</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>18xchcy</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>First time doing cuticle care and shaping my nails</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18xchcy/first_time_doing_cuticle_care_and_shaping_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>18xbiah</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Using rubber bases on top of colored gels?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18xbiah/using_rubber_bases_on_top_of_colored_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>18xb739</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Nails for the new year</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jrlmb6sr5ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>18xb2we</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>New Years Set</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xb2we</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>18xasvl</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>new nails</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upkppr92o5ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>18xaosz</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Would this be weird as a full set?</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6irnqdtym5ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>18x9ayq</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Best nail paint?</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18x9ayq/best_nail_paint/</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>18x7gvo</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>New year, new set ✨</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/09en94dyu4ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>18x68gq</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>hyponychium</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x68gq</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>18x5qfw</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Bill Kaulitz nails inspired nails &lt;3</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0i89g0yg4ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>18xabum</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>I'm in NZ and want to buy some sort of BIAB gel but worried about getting a legit product</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18xabum/im_in_nz_and_want_to_buy_some_sort_of_biab_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>18x0fs0</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>How do I get these to look less press on-like?</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x0fs0</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>18wz197</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Nail tech left a layer of acrylic - go back a 3rd time?</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18wz197/nail_tech_left_a_layer_of_acrylic_go_back_a_3rd/</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>18x9h28</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>What supplies do I need to buy in order to take care of my brittle nails?</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18x9h28/what_supplies_do_i_need_to_buy_in_order_to_take/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>18x8mgr</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>New set🖤💜</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rs8ocmuq45ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>18x8fyz</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Starsss</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x8fyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>18x8065</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>New years natural nails (one year of diy nails, feedback welcome)</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x8065</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>18x7int</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Nail progress!! God my first ones are so bad lol</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x7int</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>18x6ga0</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Painted and did my own chrome powder</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x6ga0</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>18x5u4i</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>How do these press-ons look?</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/601h0fqqh4ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>18x54qa</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Villain nails</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8apm4ocbc4ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>18x519r</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Color dupe to this</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvo3rv1mb4ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>18x4y9b</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Romantic French Mani</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xgv2nlza4ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>18x3jgd</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Mooncat Cruel Mirage</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x3jgd</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>18x2v1h</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>first ever nails</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x2v1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>18x2qt2</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>You all hate this as much as I do?(nt)</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x2qt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>18x2fo8</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Finding ways to have fun with shorties after busting a nail trying to do my toes 😭</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x2fo8</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>18x2byr</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Decided to do my fav colour again. Reminds me of glow sticks</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x2byr</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>18x26c7</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>First manicure to strengthen nails-worth it?</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18x26c7/first_manicure_to_strengthen_nailsworth_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>18x1ryf</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>90’s Angel aesthetic 👼✨</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x1ryf</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>18x1o0a</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Nail care question</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18x1o0a/nail_care_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>18x1hf0</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Went for cute nails with nail tech</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qm4trn3kl3ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>18x0rvc</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>When I let my nail tech choose the designs, she only charges me for the first two! Happy New Year!</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x0rvc</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>18x0pyp</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Why are velvet nails so mesmerizing?!</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/if8znb56g3ac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>18x0hs8</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Getting my nails done for the first time!</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18x0hs8/getting_my_nails_done_for_the_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>18x025s</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>My latest set!</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x025s</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>18wzj4w</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Gel Extensions Lifting</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18wzj4w/gel_extensions_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>18wziir</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>is nail staining more of an american thing?</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18wziir/is_nail_staining_more_of_an_american_thing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>18wyikd</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Can I use the loose glitters from my gel kit with normal nail polish?</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18wyikd/can_i_use_the_loose_glitters_from_my_gel_kit_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>18wy73d</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>am i overthinking or is this lifting? (sorry i literally know nothing about nail extensions)</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wy73d</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>18wy2fw</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Real nails growing nicely</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wy2fw</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>18wxy9d</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>New year, new nails</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wxy9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>18wxw07</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>booking a nail appointment</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18wxw07/booking_a_nail_appointment/</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>18wxu9l</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Did some gel x with star decals and gems for the new year. 🥂 no i didn’t put cuticle oil since itd just grease up the matte coat for pic.</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wxu9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>18wxdrg</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Any magnetic gel Polish recommendations in the UK?</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18wxdrg/any_magnetic_gel_polish_recommendations_in_the_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>18wx7jf</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Did these on myself last month</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y1soaa89r2ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>18wwevm</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0egu24ml2ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>18ww30q</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Dual forms</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ww30q/dual_forms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>18wvzxp</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>bare with me i have a dumb question im new</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18wvzxp/bare_with_me_i_have_a_dumb_question_im_new/</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>18wvz0x</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>New years nails 💅</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18ew3qzei2ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>18wvp55</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>~1year progress 🥰</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wvp55</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>18wvo5h</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>One year of doing my own nails</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wvo5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>18wvmtx</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>First time doing gel nail with tip</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzzc9n54g2ac1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>18wvlhn</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Y2k duck nails</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ju885tguf2ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>18wvc69</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Aurora borealis nails 😊</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49jetyqzd2ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>18wv6gb</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Do you get used to typing with long fake nails over time?</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18wv6gb/do_you_get_used_to_typing_with_long_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>18wsy5j</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>What do I use to remove nail glue? Had press on’s, which came off easily but now I’ve got glue residue. Don’t want to buff bc I’m scared I’ll remove healthy nail.</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18wsy5j/what_do_i_use_to_remove_nail_glue_had_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>18wsy09</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Been a while since I posted my nails here... 💙🖤</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wsy09</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>18wpqlf</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>My nails through 2023 💅</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wpqlf</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>18wdi8s</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Peeling off? Is this normal?</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wdi8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>18wacuf</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Nail update</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wacuf</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>18w933m</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>when nail polish is still on, but my nails are getting to long &amp; i need to file them, what do I do?</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18w933m/when_nail_polish_is_still_on_but_my_nails_are/</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>18w84yv</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Help with my nails, never grew them out before!</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18w84yv</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>18wul4f</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Seashell nails!</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wul4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>18wuk2m</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>rip</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wuk2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>18wg380</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Fake nails (press on) first timer</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wg380</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>18wt9xx</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>First time painting my nails</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b91v7fr0z1ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>18wt5kq</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>abstract christmas trees i did 💚💗</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/trnzhho4y1ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>18wt037</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Need ideas</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l88re16zw1ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>18wshbp</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Best nail shape for me?</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wshbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>18ws434</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Winter gnome set</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/077cr7f5q1ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>18wq5jn</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Totally 80s Barbie vibes for the first mani of the year. LA Colors / Fuel shimmer fuchsia under Sally Hansen / Pixel Perfect black and white geometric confetti. Let's go party.</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wq5jn</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>18wq1kh</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Weather in the UK is miserable so I brought early summer with my nails</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wlv6tyh891ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>18wpq46</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Something different for January nails!</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wpq46</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>18wpi3c</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Anyone play guitar? Finally happy with the length of my nails and it’s been difficult for my fretting fingers.</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qx4dtihf41ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>18wjtb9</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>WHY is my OPI like this?!?!</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/su1tmvw4dz9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>18woemn</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Anyone else appreciate a sheer nude from time to time?</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2a2nfi3u0ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>18wnt4g</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>First attempt at painting a character/portrait on a nail. It’s not perfect but I’m pretty happy</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjmhorf2o0ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>18wmm77</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My NY nails are brighter than my future </t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yvktbo9oa0ac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>18wmj6y</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Didn't really like them much at first, but I love them now!,</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wmj6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>18wlsij</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Got chrome for the first time and I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wlsij</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>18wlgvv</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>2023 nail recap</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wlgvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>18wkf4o</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>New Year’s Nails</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lv0ow7b7kz9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>18wkazc</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>What do you all think of my new year nails? 💅</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wkazc</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>18xdue3</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>The nail polish that got me into collecting nail polishes</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xdue3</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>18xbjtq</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Last Christmas manicure 2023</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xzl0tl8v5ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>18xclme</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Advice needed, is it normal for my nails to be this bendy?</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18xclme/advice_needed_is_it_normal_for_my_nails_to_be/</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>18xchxt</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Finally getting on the fairy dust train 🧚‍♀️✨</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gh9kwdpg46ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>18xch05</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Claw pose is all I know 😂</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f18q495746ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>18xbkbx</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>I have been crying out to you from the start</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xbkbx</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>18xafjb</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Love ILNPs packaging 💖</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0p23vkmk5ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>18x7ba8</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>mooncat mercury’s tears</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/84aw87opt4ac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>18wzjs2</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>New Year’s Nails — Happy New Year everyone! Polishes Used: Sally Hansen Miracle Gel (Shade: Onyx-pected) | Holo Taco (Shade: Play Rosé) | Seche Vite (Instant Gel Effect Top Coat)</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kyvw1aqu73ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>18x7xiw</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Started doing my own 2 months ago :)</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x7xiw</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>18x9y2c</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Velvet nail with regular polish question</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18x9y2c/velvet_nail_with_regular_polish_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>18x9pil</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Beetles Gel Polish Advice?</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x9pil</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>18x973f</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Thermal polish question</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18x973f/thermal_polish_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>18x9091</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Cirque REM vs. Holo Taco Wireless Mode</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tp4x8u0z75ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>18x8iws</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Canadian</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18x8iws/canadian/</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>18x8h52</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Recommendations for overfiled nail 😢</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/82hsr1gg35ac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>18x7m83</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Anyone else fighting for their lives during the ethereal drop</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18x7m83/anyone_else_fighting_for_their_lives_during_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>18x7j30</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>When in French Polynesia</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x7j30</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>18x7c4a</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>A sparkly start to 2024</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x7c4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>18x6ymi</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>I’m the only leftover</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nzw00p6uq4ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>18x6u0d</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>First nails of the year (I’m new here!)</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x6u0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>18x6ihh</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>My Top Coat is Pissing Me Off</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x6ihh</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>18x5xp2</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>New Year Skittle!</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x5xp2</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>18x5u15</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Been keeping my nails painted now for 1 year</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x5u15</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>18x5dby</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Zoya is doing another 10 for 25 sale</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18x5dby/zoya_is_doing_another_10_for_25_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>18x4y7a</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Press on tips materials</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3w3e8z1za4ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>18x4jhv</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>How do you get your manicures neat at the cuticles?</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18x4jhv/how_do_you_get_your_manicures_neat_at_the_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>18x46vf</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Aspiring Laqueristo - what have I missed!</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18x46vf/aspiring_laqueristo_what_have_i_missed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>18x3vk0</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>This NYE mani made me feel extra sad about chopping my talons down, but typing was getting so painful!</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x3vk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>18x2xbq</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Vintage vibes</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x2xbq</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>18x2trn</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Topcoat for toenails</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18x2trn/topcoat_for_toenails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>18x2s4r</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>This is not the direction I was planning on going today but here we are...</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4xw181su3ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>18x2d18</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Finding ways to have extra fun with shorties since I busted one in the process of doing my toes 😤</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x2d18</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>18x27nd</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Essie Lilacism + Blanc</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vg6o62fmq3ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>18x1zbc</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Anybody else disappointed by HT Black Holo Wish?</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0xpnduzo3ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>18x1uhy</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Has anyone ever tried using clear nail polish as a (poor) substitute for nail glue?</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18x1uhy/has_anyone_ever_tried_using_clear_nail_polish_as/</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>18x1ltr</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>first Emily deMolly order didn’t disappoint!</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x1ltr</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>18x1ckn</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Essie Gel Couture Top Coat shrinkage?</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x1ckn</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>18x19lb</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Resolved to be kinder to my nails this year</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a71ggw61k3ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>18x16dg</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>had to say goodbye to the square shape 🥲💚</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9kx3y5sej3ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>18x0z0k</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Not really Impressed</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18x0z0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>18wxpsl</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Londontown sale issue</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18wxpsl/londontown_sale_issue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>18wzpct</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Comet by ILNP is so shifty!</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wzpct</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>18wzm7c</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Something simple and sweet - counting down the days until winter is over</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wzm7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>18wzgk9</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>HOH truly glows!!</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5fmdj6573ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>18wzdum</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Moody shiftiness for winter</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wzdum</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>18wzcwh</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Posted this yesterday, didn’t think my nails did the color justice, deleted, but reposting after compliments today. Shoutout to Winter Is So Chill from Bluebird.</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zok33ifh63ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>18wyt61</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>New Year Nails!</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wyt61</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>18wy9ey</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>sorry if someone has already posted this here, but this advertisement stopped me in my tracks this morning!</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1iqgra3ry2ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>18wxzo7</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Loving the Holo shimmer!</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebzt7vdpw2ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>18wxyui</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Swatching everything I own so far was an unexpectedly joyous occasion! 🥹</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wxyui</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>18wxu6y</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Anyone had luck with this kit?</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zi8fnrqv2ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>18wxrye</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Bought These at my local Target for $2.99-$4.29 USD</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3cco4gaav2ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>18wx4yn</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>my year of polish!</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wx4yn</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>18wwuqe</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Did I buy a polish just because of it's name.... maybe... but I really do like the color and glitter!</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wwuqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>18wwq8i</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Starting off the new year with a fully swatched, sorted, and numbered polish collection! And a bonus photo of my NYE mani 😁</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wwq8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>18wwbre</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Took my bottle of Mooncat Ghosts of Hecate to the manicurist</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wwbre</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>18ww7z4</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>My snow globe nails ❄️</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujofgyi8k2ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>18ww6wf</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>This polish in the sun. 🤌</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ww6wf</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>18ww5xh</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NYE mani, bring on the sparkle! Outfit in comments </t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fzen03gtj2ac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>18wvqfr</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>How are the formulas on Blank Beauty custom cremes?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18wvqfr/how_are_the_formulas_on_blank_beauty_custom_cremes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>18wvl0f</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Similar holo in other ILNP polishes?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nn8frdxqf2ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>18wv6l8</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>First mani of the new year!</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4y23wfvc2ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>18wv0ov</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>“Love the One I’m With” or buy new??? LED lamp</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/27jdr22sb2ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>18wukul</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>HT Peach Tea and Mooncat Fake Halo</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wukul</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>18wotsw</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>First polish of the year. From base to top -OPI Nail Envy -Essie smooth-e ridge filler -OPI infinite shine Linger Over Coffee(2 coats) -Glisten &amp; Glow top coat</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wotsw</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>18wujgs</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Mini swatch for Nov/Dec pickups</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wujgs</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>18wt91t</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Winter Vibes ❄️</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wt91t</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>18wt7j5</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Canadian Girlies</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18wt7j5/canadian_girlies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>18wsvyh</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>My fave polish of 2023 goes to…</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wsvyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>18wsr9k</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Airport Security Stole My Nail Polish</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18wsr9k/airport_security_stole_my_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>18wseey</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Not sure how I feel about these. Kind of giving lizard/frog vibes 😅</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1t201w4fs1ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>18ws90p</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>First time doing a jelly sandwich with Cirque colors!</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hb5qii9r1ac1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>18wrhcn</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>🐉🐉</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wrhcn</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>18wqguk</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>🍽🌈Fiestaware 🌈🍽</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wqguk</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>18wq7km</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>First nails of the year ✨️</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ccdfz2uia1ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>18wke30</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>First nails of the year is a blast from the past</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wke30</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>18x0sk7</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Why are velvet nails so mesmerizing?!</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dg67l15pg3ac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>18wvoh6</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>50s diner inspired</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wvoh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>18wsb9x</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>First time trying a jelly sandwich!</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlrcnviqr1ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>18ws2h5</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Winter gnome nails</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w3q6fctsp1ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>18wlhd6</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Diving into matte</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18wlhd6</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jan  4 08:08:08 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_07.xlsx
+++ b/data/2024_01_07.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C610"/>
+  <dimension ref="A1:C768"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10803,6 +10803,2692 @@
         </is>
       </c>
     </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>18y7wc1</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>I like to call this colour “gunmetal pink”</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y7wc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>18y7tqt</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Does anyone else do mismatch sets? Lol</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y7tqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>18y7n1d</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>recent set</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y7n1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>18y7hz5</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>What nail are these</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0iqksh59ndac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>18y7d3u</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>My favourite set to date</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfis0rjoldac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>18y6rxm</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>The vision vs the end result</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y6rxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>18y4isp</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>First nail look of the year ✨</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y4isp</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>18y4ifa</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I had to reupload due to some type of quality issue but I worked really hard on these during a particularly hard time to keep myself busy. This is completely unedited, they just really are that vibrant! Thank you guys for the support on my last post, really appreciate it. </t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zrjxa992scac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>18y44r5</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Tips for starting out for a disabled person?</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18y44r5/tips_for_starting_out_for_a_disabled_person/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>18y3etd</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>I think this was my best set so far…</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqfr2ug2icac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>18y3bj0</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Last year's nubs vs latest growth</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y3bj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>18y36zb</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>my trademark color ♥️</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flkb9fw3gcac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>18y2k1f</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>How safe are these chrome powders?</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7otzbakkacac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>18xzs62</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Under nail care?</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18xzs62/under_nail_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>18xtslg</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Little Twin Stars Nails ✨</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwymjix8gaac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>18y2ghj</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Hand-painted cat nail art by me. Finally had time to do my own nails. Drawing with the non-dominant hand is really challenging. Any cat people here?</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i8v6h2tq9cac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>18y29r6</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>What is your favourite black acrylic nail powder</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18y29r6/what_is_your_favourite_black_acrylic_nail_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>18y21tv</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>✨Matte white nails ✨</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nvcuw2ta6cac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>18y1yed</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Love this polish!</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hdkdl64i5cac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>18y1vmm</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>first time getting chrome nails</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y1vmm</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>18y1h33</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Paid $90 for these. I like them but idk a lot on nails. How do they look to you guys?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y1h33</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>18y14n0</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>more star nails! this time on my natural nails</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y14n0</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>18y0wc8</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Color combo sparking joy 💜💗</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z364so8xwbac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>18y0a5e</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>My fav set</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y0a5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>18y07q1</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Is it too soon?</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18y07q1/is_it_too_soon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>18y07pj</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>How often do you get your nails filled?</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18y07pj/how_often_do_you_get_your_nails_filled/</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>18y01rx</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Messed up those retro 80s nails yesterday by not properly sealing the confetti so today it's NuColor 973 (their polishes don't have names) topped with LA Colors Vivid Blooms.</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y01rx</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>18xzsed</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>1st set of the year</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hy4txwf5obac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>18xzpmb</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Made some press on's!</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j0f9rmbjnbac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>18xzaf6</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>I removed my gel polish and my nails still have the base coat on, they look brittle and damaged. Before getting the gel polish, they were great and strong. Any advice?</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mstsd6bkbac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>18xyuym</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Pearl chrome powder nails</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zfl6a900hbac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>18xy4uv</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>I adore my nail tech! Scooby-Doo for the win!</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/seidwezjbbac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>18xy4ah</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Jeweled 💙🌸</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j388uucfbbac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>18xy3pj</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>One year progress pics</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xy3pj</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>18xy0c2</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Can you use chromatic pigment powders on normal nail polish</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18xy0c2/can_you_use_chromatic_pigment_powders_on_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>18xxs8j</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>new year, new nails</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpzjlr8z8bac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>18xxbsr</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Still in learning Progress. My First Time doing it without tips. Took me 4h. (15y)</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xxbsr</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>18xx0xg</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Cloudy nights ☁️🌙</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hz7a4rsh3bac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>18xwcix</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Favorite sets I've done in 2023 ✨</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xwcix</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>18xw8ap</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>my tech really outdid herself with these whimsigoth nails</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xw8ap</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>18xw10s</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>do these press one suit me?</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xw10s</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>18xvsdn</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>You can do it, just keep practicing 💪💅❤️</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/td0r6wvluaac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>18xqngb</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>nail ideas anyone?</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18xqngb/nail_ideas_anyone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>18xpiuo</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>silver nails 🩶✨</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xpiuo</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>18xvqo2</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>My nails over the years</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xvqo2</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>18xskba</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Turns out I'm allergic to vegan nail paint, please help.</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18xskba/turns_out_im_allergic_to_vegan_nail_paint_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>18xvmq7</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Cateye nails</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r49ujsogtaac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>18xv9gd</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>2D Pop Art style</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9v97g5buqaac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>18xu62y</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Ballet themed and super easy!</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xu62y</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>18xtzni</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>What did I do wrong?</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h8mrldpnhaac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>18xto85</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xto85</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>18xtdw3</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>anniversary nails 🤍💕</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xtdw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>18xtd4c</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Opi onyx black and Northern lights</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xtd4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>18xsufs</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>First time doing my own gel x extensions</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xsufs</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>18xsonl</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>I love this blue, and you? I don't think it's a very popular choice of colour.</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3dnt8268aac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>18xsll6</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>all my BIAB sets beginning from feb 2022 until now :)</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xsll6</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>18xse8u</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>When to get fills vs full sets?</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18xse8u/when_to_get_fills_vs_full_sets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>18xrvet</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Soft Celestial</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1apmubf2aac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>18xrdy6</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Is there any way for me to save my (gel) nail art!</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tbgb02b1z9ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>18xrdb4</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>My vacation nails 🍒</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qxwcbcgwy9ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>18xr09f</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Question about pre-painting gel nail tips</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18xr09f/question_about_prepainting_gel_nail_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>18xqt2l</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>My Dad is Looking for Anti-Bite Polish</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18xqt2l/my_dad_is_looking_for_antibite_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>18xqbkp</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Manifesting strong natural nails for everyone this year</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xqbkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>18xq4rx</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>i started doing gel-x nails in june of 2023, here are some of the sets i did last year ❤️</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xq4rx</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>18xpxkf</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>I could’ve shaped better but I’m obsessed I think these are the cleanest nails I’ve done for myself. Gel overlay.</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6mqn0bro9ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>18xpnjg</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Went for icy vibe, with pink shimmer (I don’t think I like the rhinestones on my one thumb 🙈)</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xpnjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>18xpeez</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>I did nails for my GF. First time ever doing gel nails.</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xpeez</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>18xpe3f</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Sparkly noodz for the new year 💖</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/97mq7guxk9ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>18xp4yt</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>did my own nails. thoughts?</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xp4yt</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>18xoxhh</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>First time getting acrylics</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xoxhh</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>18xis9y</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Trying again to grow my nails - advice needed!</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ax0874e038ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>18xn078</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>What shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xn078</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>18xmysy</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Milky candy 🍭</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b5i8d5pl19ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>18xmfsr</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>🩷🩷</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k40vloylx8ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>18xm5r9</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Lapis of Luxury</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xm5r9</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>18xlz8m</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Love a ‘simple’ mani</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xlz8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>18xlfrw</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>OPI press-ons (long in color “alpine snow”)! 💟</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xlfrw</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>18xlevj</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Paid $65 for these. First time getting acrylics done at a salon.</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xlevj</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>18xl8lg</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>My NYE nails</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ww58oxn7o8ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>18xl887</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>DIY nuance nails</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8847ngu4o8ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>18xk84x</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>New year new nails</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4jazeytf8ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>18xk2ue</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>My January set</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/de14viele8ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>18xizde</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>press ons</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y2naxeso48ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>18xim1k</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>A dad on a mission, I've struggled with stars since I was a kid.</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xim1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>18xih01</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>First time having my nails done...</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bandyggxz7ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>18xhvyt</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>The third day of the year and good nails</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4ppn933u7ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>18xf6sk</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Has anyone done pink nail polish with gold chrome powder, or gold nail polish with pink chrome? I’m not sure if my vision will look the way I hope or not, and would love to see pictures.</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18xf6sk/has_anyone_done_pink_nail_polish_with_gold_chrome/</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>18xf5e3</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Is 3mm of nail growth over the course of a week fast or slow?</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18xf5e3/is_3mm_of_nail_growth_over_the_course_of_a_week/</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>18y77ys</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>I didn’t think I was a bright pink person, until now</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y77ys</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>18y6qd6</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Mooncat’s Firewall Dupe?</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b4sdij0hedac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>18y5hw8</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Thank y’all for putting me on to better products</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4z8h1ki1dac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>18y3w9y</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>I don't want to ruin my boyfriends nailbeds</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18y3w9y/i_dont_want_to_ruin_my_boyfriends_nailbeds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>18y3rho</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Some late New Year's nails!</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y3rho</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>18y2xrz</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>First manicure of 2024 and she’s a sassy one</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y2xrz</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>18y2f39</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>“Yeah, hi, how much for an extra thumb?”</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4k3k9oug9cac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>18y2618</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Does anyone notice that polish takes longer to dry at night or is it just me?</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2wa2qtma7cac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>18y22x8</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Fluorescent bus lights are perfect for showing off A Midsummer’s Dream😍</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y22x8</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>18y1ez8</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>First mani of 2024!</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46emvxo11cac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>18y0xx2</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Abracadabra</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y0xx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>18y0e74</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Ignore my soup, I’m sick lol</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y0e74</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>18y08pt</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Just got Cirque Hatch, new immediately I had to pair it with Morningtide for glazed stoneware nails</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y08pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>18xzy5y</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>[Beginner] Any reason I SHOULDN'T change my nail polish every day? Including yesterday's mani</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqb9g9bdpbac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>18xz3ap</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Surprising 😍</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xz3ap</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>18xyvxx</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Polish Thinner</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18xyvxx/polish_thinner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>18xrwi6</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>A little icy blue for January with a touch of unicorn magic ❄️🦄✨ Polishes Used: Lights Lacquer (Shade: We Were On A Break) | Holo Taco (Shade: Cosmic Unicorn Skin) | Seche Vite (Instant Gel Effect Top Coat)</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eyc05mxm2aac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>18xtptt</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Proud to stop picking my cuticles. Keeping it simple, love this colour for winter!</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ow9gu2xofaac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>18xw8jv</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>I took a pic "with the claw". RIP Miss Chanandler Bong.</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fa6dcdwuxaac1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>18xw3qv</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Best budget top coat 🙏🏻 not sponsored, just need to put ya’ll onto this!!</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mltvvkmwwaac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>18xvmqx</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Help! Seeking Lacquer Thinner Tips</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18xvmqx/help_seeking_lacquer_thinner_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>18xvhxc</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Newbie question</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18xvhxc/newbie_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>18xuqxt</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Polished For Days Interstellar</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yecq3ra4naac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>18xue2f</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Starting the year off with Shooting Star!</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xue2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>18xu918</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Icy blues</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqxn1xojjaac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>18xtte3</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Back in the workshop with more Lyn B, this time featuring paduk</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xtte3</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>18xt9sd</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Zoya Betty + BKL To Teach Us About Our Past</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xt9sd</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>18xt4km</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>What the Hecking Heck?!?</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xt4km</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>18xt14v</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>This polish has no right to be this pretty!!</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xt14v</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>18xswv4</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Blue Nails</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xswv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>18xssj6</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>New Year nails. Broke a bunch renovation but been not picking anymore</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5uvbpyy8aac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>18xsgez</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>1st Death Valley Nails order 🤩</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55ueuhsk6aac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>18xse5b</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>These feel so good 💅🏻</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9g3i89y26aac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>18xry7j</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Zoya 10 for $25 is back!</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcimq7oy2aac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>18xrw5z</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>3 years since I used this color!</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggitq3lk2aac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>18xqq46</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Flower jellies 🤤</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xqq46</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>18xqibn</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Is brown my color?</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xqibn</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>18xq7y9</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Best base and top coat?</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18xq7y9/best_base_and_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>18xpx6r</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>OPI repair mode</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18xpx6r/opi_repair_mode/</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>18xpsne</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>new year new me</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xpsne</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>18xppiu</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Holiday leftovers: red skinny french!</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xppiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>18xpl95</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>💙🩵🌤Blue Skies🌤🩵💙</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xpl95</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>18xof6b</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Polish decant supplies</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18xof6b/polish_decant_supplies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>18xobly</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>How do I get the rest of this gel off without destroying my nails?</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7us3t85cd9ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>18xnhz8</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>First mani of 2023 (belated): brilliant, bright, and goddamn GLOWY 🌌✨</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xq0eo8k59ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>18xmuc6</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Quick Fix...</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0h1tiqjo09ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>18xmq62</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Lavender love</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xmq62</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>18xmei9</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Has anyone tried Glisten &amp; Glow’s hand and nail nutrition?</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18xmei9/has_anyone_tried_glisten_glows_hand_and_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>18xmbtm</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>✅ colour ... 🚫 formula</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xmbtm</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>18xm7ir</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Lapiz of Luxury</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xm7ir</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>18xlymx</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Fairy dust lives up to the hype!</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xlymx</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>18xlydh</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>I love a ‘simple’ mani</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xlydh</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>18xlnfn</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Nails Inc x Percy Pig</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xlnfn</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>18xlfju</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Help with damaged nails after extended gel wear</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18xlfju/help_with_damaged_nails_after_extended_gel_wear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>18xkun6</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Appreciation post for Lestat</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xkun6</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>18xk3nl</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>How does one tell if they received a "bad batch"?</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18xk3nl/how_does_one_tell_if_they_received_a_bad_batch/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>18xj3kc</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>A bit of a sparkly palette cleanser 😘</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4nbbgzyw58ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>18xi7my</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>{PR} Jet Setter by ILNP 🎆🎇</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1jtpq3ex7ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>18x17zs</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>When your nails are on point and....</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1b41xqpj3ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>18y521n</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Short gel nails 🌸</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ws2cfcb7xcac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>18y3pac</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>new year, new me</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ioy09omkcac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>18y2tre</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Simple Valentines Day Nails</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y2tre</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>18y24ff</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>some of my favorite seasonal nails I’ve done, all hand painted by me</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y24ff</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>18y0bdm</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>💚</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y0bdm</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>18xzncg</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>How are you all so dang good at this stuff..</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18xzncg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>18xykb9</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Question: How do I seal chrome powder with top coat, since the top coat brush gets glittery??</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/18xykb9/question_how_do_i_seal_chrome_powder_with_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>18xxusu</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Gel X lavender cowprint to kick off the birthday month ✨</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xflimuyi9bac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>18xvkkx</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Christmas - charms on gel by Black Orchid Salon Amsterdam</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzsvywo1taac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>18xuvph</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Little Twin Stars Nails ✨</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqgt6jz2oaac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>18xpjjh</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>blood effect 🩸💉💉For my client today 🥰</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xaw8kr8yl9ac1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jan  5 08:08:06 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_07.xlsx
+++ b/data/2024_01_07.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C768"/>
+  <dimension ref="A1:C926"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13489,6 +13489,2692 @@
         </is>
       </c>
     </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>18z1fin</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>New year, new nail!</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18z1fin</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>18z04do</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>My favorite sets I did in 2023</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18z04do</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>18z020o</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Glitz Adora</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1q6p5nkekac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>18yzqk2</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Scooby doo glow in the dark nail😁 second time painting a character on a nail</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yzqk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>18yzgea</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>simple set🪩💿</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yzgea</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>18ylc5v</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>First polish of 2024 matches my boyo's toe beans 🩷</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ylc5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>18yhwfr</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Looking for wedding nail inspo</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18yhwfr/looking_for_wedding_nail_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>18yyglj</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Gel nail polish peeled off</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18yyglj/gel_nail_polish_peeled_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>18yy90d</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Please help!</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yy90d</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>18yy5mc</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Natural nails progress</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yy5mc</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>18yxpko</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Will nail polish with no acetone remove gel polish?</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18yxpko/will_nail_polish_with_no_acetone_remove_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>18yxl8x</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Got acrylics for the first time by my bf's 14 y.o sister</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yxl8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>18ywjnc</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Still one of my fav polish colors</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqdjbhnihjac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>18ywit5</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Poly Gel Newbie. Any tips and tricks so my nails aren't so unpleasant looking next time?</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0b92syahjac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>18ywg2l</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>new years nails for my sister (she took the pics herself bc i forgot)</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtw7yqumgjac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>18ywdsa</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>What should I do?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/if4zmxa3gjac1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>18ywc8k</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>I feel like I robbed my salon</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5rcraopfjac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>18yvpp1</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>💙 for January</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fjvzliuhajac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>18yunnp</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Bring my own polish?</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18yunnp/bring_my_own_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>18yujsn</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>New set for 2024</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/491otgdmziac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>18yu2fs</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>[UPDATE] Paid $65 for these. First time getting acrylics done at salon.</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yu2fs</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>18ytfw3</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Milky white nails 🥛</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ytfw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>18ytaap</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>NEW SET! I love my life rn!</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ytaap</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>18yt68c</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Chamaeleon Nails - Daryl's Hunt (thermal)</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yt68c</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>18yt0za</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>new set of nails! super simple ^_^</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yt0za</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>18ysay2</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Nails grow uneven</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxax8qkziiac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>18yqpqk</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jpvja5r57iac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>18yqoxd</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>I haven’t gotten my nails done in years. I’ve been feeling really down and I wanted to cheer up. A simple French manicure felt like a good place to start.</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldzwornz6iac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>18yq8i6</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>My first go at polygel nails</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qh5c7b2p3iac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>18ypvlg</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Gel x popping off - help!</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ypvlg/gel_x_popping_off_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>18yprzz</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Blue chrome 💙</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yprzz</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>18ypdaz</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Thoughts on nail art like this?</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3sinrmsxhac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>18yp6oq</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Soft abstract set</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yp6oq</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>18yove6</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>advice needed</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yove6</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>18yojls</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Olive &amp; June Press-ons!</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/spl957arrhac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>18yogxy</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>I need help with my cuticles…</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18yogxy/i_need_help_with_my_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>18yogs3</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Why can't I buy nail-aid anywhere?</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w3n264v6rhac1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>18yoceh</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Milkyyy</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yoceh</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>18ynxyp</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>I used to suffer with severe mental health issues, I used to rip my nails off, I'm growing them back and filing them to make them pretty, not amazing but I'm happy to be trying :)</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hyw2eajcnhac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>18ynvp0</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>First set of 2024! 🍒</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bbc1vvlvmhac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>18ynkve</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Milky white 🤍 ✨</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ynkve</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>18ymuq1</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Got yellow under my fake nails!</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ymuq1/got_yellow_under_my_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>18ymocn</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Obsessed with the glitter!</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0yjyshgxdhac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>18ymlyc</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Yes or No?🩷🩵💚🧡💜</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sfggnvjfdhac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>18ymh9a</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Poly gel nails + gel nail polish</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ujadimgchac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>18ym9lk</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Help please! Can this be fixed or should I get new set?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ym9lk</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>18ylv1z</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>This color is just something, the manicure is done very neatly, I like it</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29eou1218hac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>18ylnrl</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Can’t tell if I love these valentines geode nails that I did</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdu86y6n6hac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>18yljsa</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>My sister was my nailtech. She died of an OD on dec 14th. She was 22. My first attempt at doing them myself.</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9kh1owt5hac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>18ylhha</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>✨✨✨</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3bccbdc5hac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>18yl6h8</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Tips to use under gel polish</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18yl6h8/tips_to_use_under_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>18yk62f</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Does anyone else do mismatch sets? Lol</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yk62f</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>18yjzhd</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Does this nude base match me? Also, what can I do to prevent/limit chrome rubbing off prematurely? (Structured Mani)</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4rw5wc3kugac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>18yjx0r</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Has anyone tried this viral nail glue???</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebe72za2ugac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>18yjtch</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>New nail goofin</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yjtch</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>18yjpe2</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Before/After getting a professional manicure for the first time</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yjpe2</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>18yjcm2</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Very proud of these nails I did</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yjcm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>18yjc6c</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>New manicure</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibr78grwpgac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>18yjaao</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Simple frenchie for 2024</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvbqzg8ipgac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>18yiso9</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>I just can’t get enough of this color, shape and sparkle!!</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yiso9</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>18yihyj</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>New nails for the new year 💕</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d0qcuuapjgac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>18yi7nq</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Went out of my comfort zone, and I’m totally obsessed. Still in shock that these are my real nails.</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58ea5s5lhgac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>18yi500</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Why do nail techs up-charge some clients but not others?</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18yi500/why_do_nail_techs_upcharge_some_clients_but_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>18yhvwk</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Mysterious and sparkly</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ab0l9t07fgac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>18yhvbv</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Lunlula on nail</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8y51rt2fgac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>18ygutq</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Do you get a manicure/cuticle trim when getting a fill?</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ygutq/do_you_get_a_manicurecuticle_trim_when_getting_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>18ygtu7</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>🥀✨</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l46a0tja7gac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>18yglyf</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Should I keep this shape or try something different?</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhur5hdn5gac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>18ygjl7</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Shorties</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pf22obk55gac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>18yf818</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Why do my nails keep splitting like this?</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vbmp96jqufac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>18ydf7i</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Is there anything I can do to stop my nails from growing upwards?</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ydf7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>18y8gc8</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Having issues with nail polish and upkeep</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18y8gc8/having_issues_with_nail_polish_and_upkeep/</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>18yeza1</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>First set for 2024</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ng0zv6ssfac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>18yekhp</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>New nails 😍</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yekhp</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>18yeicz</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>I’m not sure how to ask for what I want!</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kyy4a1mvofac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>18ye873</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>My most favourite manicure</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gf6qz8xgmfac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>18ycnn5</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Disney Nails</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ycnn5/disney_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>18ycjft</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Manage my time and increate productivity</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ycjft/manage_my_time_and_increate_productivity/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>18ybhwf</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>New year’s classic me…starting with my nails</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4kgonsuxeac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>18yb79s</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Polygel</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g59ajeoqueac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>18yaxog</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Good gel brands in the UK?</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18yaxog/good_gel_brands_in_the_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>18yav09</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Haven’t done my nails forever</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mag1xdp1reac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>18yame1</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Metallic (grudge) nails</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yame1</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>18yals2</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Didn’t like them at first but now I can’t stop looking! So in love with this set</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yals2</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>18yaj44</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Take 2? 😆 I need picture taking tips apparently. Sorry for the shiny background last time guys! 😆 ❤️</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yaj44</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>18yadfu</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>I painted my natural nails a pearlescent white to match my pearls</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rhe2pknleac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>18yacsr</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Did something out of my comfort zone for 2024</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nw412ewgleac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>18y9soo</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Any non toxic nail recommendations?</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18y9soo/any_non_toxic_nail_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>18y9ben</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Tried to do a French mani on myself for the first time. Feedback would be appreciated :)</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lazfr7x69eac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>18y8tjp</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Pink Christmas. Better late than never ☺️</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26w3zk493eac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>18y8qmn</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>First time at-home nails</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y8qmn</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>18y8mtv</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Almost 2 months since I started. I want to be a nail tech soooo bad</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9oe6s4gz0eac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>18y8l4e</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>First time going to an independent artist</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6etp0ud0eac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>18y8dqx</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Love how this turned out🥹 practicing with isolated chrome and sculpture gel</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y8dqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>18y8dqv</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>How did I do? I really like them!</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bzbr409uxdac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>18y7yz8</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Did these forever 😰</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/44i7h03usdac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>18z1302</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Shopping my stash on PPU eve</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18z1302</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>18yh24q</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Sassy Sauce thermal color change</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkx05wdx8gac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>18yxivp</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>First mani of 2024</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgxhv6bcqjac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>18yxe4l</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Cirque Chemistry (Velvet Effect)</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tmblf543pjac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>18yx5ll</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>What is your favorite white?</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yx5ll</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>18yx44i</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>KBShimmer on Etsy</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18yx44i/kbshimmer_on_etsy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>18ywxsg</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>ILNP Nostalgia 🪲</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ywxsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>18yw3sb</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>One more in dark lighting</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7pl9t0tdjac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>18yvwge</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Light Pink French Gel with Chrome 🥰</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yvwge</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>18yvpio</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Good from far</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tr0c7hcgajac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>18yvdzr</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>So I know a lot of people dislike mystery bags…</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18yvdzr/so_i_know_a_lot_of_people_dislike_mystery_bags/</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>18yt8m8</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Chamaeleon Nails - Daryl's Hunt (thermal)</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yt8m8</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>18yt1cs</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Favorite of 2023 goes to Midsummer's Dream 🧚🏻‍♀️✨</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7s04jbkoiac1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>18yrzek</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Polishes I’ve worn in the last month</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yrzek</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>18yrvbq</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Will someone please help me?</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k7g6b64tfiac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>18yro8k</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>When you're sick in bed and need to feel extra</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yro8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>18yro2l</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Something between ILNP's Sweet Pea and Sandy Baby?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18yro2l/something_between_ilnps_sweet_pea_and_sandy_baby/</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>18ypzke</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>PSA: this is my opinion about the way that the Cadillaquer advent calendar was advertised and sold.</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ypzke</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>18ypyd1</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>PSA - Just made my first post and was already followed by a creep.</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18ypyd1/psa_just_made_my_first_post_and_was_already/</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>18ypp7i</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Just in case you needed confirmation that Cirque Flaminglow and Fandango are basically identical…</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ypp7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>18ype00</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Grape Expectations</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ype00</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>18yoyjx</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>First mani of 2024 🎉</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pmk8d99uuhac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>18yo3n0</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Alternative to gel nails</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18yo3n0/alternative_to_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>18ynbtj</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>All this work to be ruined by air bubbles!</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hvotbbtihac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>18ylv52</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Impressed by L.A. Colors</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgbqn9s48hac1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>18ylutu</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Ok, which one of you has my Glisten &amp; Glow order?? 😹</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18ylutu/ok_which_one_of_you_has_my_glisten_glow_order/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>18ylpw5</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Reflective Glitter: Sunlight vs Flash ✨️</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8glaqg737hac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>18ylpm2</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>The many shades of ILNP’s Undenied</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ylpm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>18ylhgb</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Magnetic nailpolish recommendations?</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ylhgb</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>18ylcyc</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>First Time Trying Great Lakes Lacquer</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2a0djjf4hac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>18yl6vq</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Please mourn with me. I never even got to use her!</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51j41qg73hac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>18yka1o</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Purple black and gold stamps</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3v8fhu8nwgac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>18yjs31</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>My collection (top row) vs my Mum’s 😂</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0vxlujk2tgac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>18yjpxi</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>garden path lacquers - i forgive you</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hzqw3nemsgac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>18yj5co</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Midnight Spark</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yj5co</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>18yixl2</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Me: my nails are slightly stained, need to give it a break. Also Me: These two deep blue shimmer shades need a comparison NOW</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yixl2</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>18yilbh</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>tfw when you forgot to topcoat just one nail 🫠</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tzz1jlddkgac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>18yihev</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Can I use UV Gel top coat over a regular polish/main to make it last?</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18yihev/can_i_use_uv_gel_top_coat_over_a_regular/</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>18yi6n7</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>You guys there is a Zoya SALE - 10 for $25 including shipping!!</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yi6n7</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>18yhvsg</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>First time doing a structured gel mani, how’d I do?🥲💕</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0n66jj6fgac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>18yhuto</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Fair Isle more like "feral" amirite</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yhuto</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>18yh3s2</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Snow Holding Back by OPI</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/en62wimc9gac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>18yguiy</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Airport nails 💅</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yguiy</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>18ygud3</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>They're not the same, they're *similar* 😅</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7gdkufe7gac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>18ygs1w</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>The true definition of insanity? This month is *trying my nerves* 😵‍💫</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lkggmkuw6gac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>18y4lqy</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Stamping Pros</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18y4lqy/stamping_pros/</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>18yer9f</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>A jelly on rounder nails makes me feel sophisticated and clean. What shape/style does that for you?</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6yu3741zqfac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>18yed42</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>So obsessed</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fjjsrs1onfac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>18ycuz5</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Icy pink for an upcoming snow this weekend</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/br2twarqafac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>18ycaf0</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Best blue in my collection 💙</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ifwiuuwi5fac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>18y9w70</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Polygel saved my nails?</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18y9w70/polygel_saved_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>18y9iak</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Some mix &amp; match chrome nails🦎✨️</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zh2d084ibeac1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>18y82f1</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Stunned seeing this polish in direct sunlight for the first time after a few days of storms and overcast skies</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pd9iuygytdac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>18ysz31</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Experimented with metallic eyeshadow ✨</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1e7m71e3oiac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>18yrhiz</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>I love minerals and stones, I've been trying to replicate my favorites with gel. Here are a few jade nails with different techniques. What do you guys think, I would love any advice</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3a3zg4wpciac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>18yp8oz</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Soft abstract set</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yp8oz</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>18ylh4f</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>I can't stop staring at my nails</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ylh4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>18yjdu9</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>I recently started doing nail art in 2023. I worked SO hard on these, over the course of 2 days. And probably used well over 10 different products to get here. I’m not sure if I chose the right flair for this.(Decided to post them in this subreddit instead! It’s a lot more laid back over here.)</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iioda3h6qgac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>18yj5pe</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Since coquette has been sll the rage.............. (done by myself)</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18yj5pe</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>18yha7i</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painted dancing Toothless from tiktok on my nails because I'm Scottish. SCOTLAND FOREVER </t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8qp62xaoagac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>18yffd6</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>New Years Nails</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14pzlafewfac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>18y8mop</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Working with isolated chrome art and nail gems ✨*beginner*</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18y8mop</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jan  6 08:07:15 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_07.xlsx
+++ b/data/2024_01_07.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C926"/>
+  <dimension ref="A1:C1099"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16175,6 +16175,2947 @@
         </is>
       </c>
     </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>18zv1ch</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Advice please</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hopsghd61sac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>18zuv22</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Do you apply Out The Door top coat on dry nails or on wet nails like Seche Vite?</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18zuv22/do_you_apply_out_the_door_top_coat_on_dry_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>18zumfe</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Marble x cat eye / marble sets that I made recently</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zumfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>18ztmtz</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Looking for Dupe of Hard Candy Crush on Lava</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1m12imidlrac1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>18ztjqq</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Are these too thick?</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ztjqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>18ztbxw</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>fresh press ons. what does everyone think??</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fj53wdo6irac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>18zspyb</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>First 2 attempts at gel extensions on practice hand/finger</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zspyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>18zsjh6</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>What's going on with my cuticles on my index finger(shortest nail in photo)?</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mw49czp6arac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>18zs6lz</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Do these make my fingers look slimmer ? (The goal) lol I always thought I had sausage fingers</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zs6lz</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>18zqvyz</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>New set! 💅🏿💗✨</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ysz4xfm7uqac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>18zqurj</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Getting better with polygel</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zqurj</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>18zqehd</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>The moment you spent HOURS on them, like them a lot, go to take pic only to realize a dog hair is permanently trapped in them. 😡😡😡😡</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nij4h20spqac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>18zq0la</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>My fiancé picked my nails for his birthday</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7aezpt49mqac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>18zq0l9</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>made by myself ❤️</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zq0l9</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>18zpr4q</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>My at home gel nails start chipping and peeling within days, what am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18zpr4q/my_at_home_gel_nails_start_chipping_and_peeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>18zhwa2</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Developed a HEMA allergy and I am so upset</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18zhwa2/developed_a_hema_allergy_and_i_am_so_upset/</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>18zi2ie</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Recommendations for Beginner At Home</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18zi2ie/recommendations_for_beginner_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>18zkspx</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>How do I take my press on off without damaging my nail?</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgxujsf6gpac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>18zltuf</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Gel X</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4i4kwpsnpac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>18zpdbu</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>My engagement nails!</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zpdbu</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>18zp74f</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Anyone know any dupes for Manicurist’s Active Glow Nail Care</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18zp74f/anyone_know_any_dupes_for_manicurists_active_glow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>18zp1li</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Second set done by myself, they are good enough for me, thoughts? Tips? These are acrylic and reg polish</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zp1li</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>18zoq34</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Recent sets by my wife at our salon</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zoq34</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>18zooxh</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>First time using magnetic nail polish 💅</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0vi2xuvaqac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>18zolkh</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Am I being too picky? It got on my cuticle and some are a little bumpy…</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zolkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>18zoala</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Are almond nails “out”</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18zoala/are_almond_nails_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>18zo90i</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Beginner- please critique and advise before I do my right hand</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zo90i</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>18zo3hc</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>i did a set of sanrio my sweet piano gel-x nail extensions on myself! i love them 🎹🕊️💕🍰</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zo3hc</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>18zo0wj</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>First compliment from someone other than my mom!</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/em712ntc5qac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>18znunh</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Short nails to start the year!</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ev06i28x3qac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>18znmpr</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Should I keep almond next time, or go for square/coffin?</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r3l2rghw1qac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>18znk72</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>LF Nail Advice</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/beauty/s/0EjyRMGyhu</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>18znihw</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>First set of the year 🌈☁️</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qagxbub51qac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>18zngvq</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Pearly romantic date night nails</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7eopdmr0qac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>18znbpd</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Lavender champagne gels for the new year. I’m pregnant so this is the only champagne I get! 🥂</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3af9q5kzpac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>18zmdue</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Just discovered this subreddit 👋🏼 Thought I would share my favorite set from 2023</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5skcfvu1spac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>18zmdav</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Mardi Gras nails, carnival season starts tomorrow 💜💚💛</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78j5zyqxrpac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>18zlfiq</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>White flames with orange chrome 🔥 (and my little sunloving orange Chi🥹)</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zlfiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>18zlen3</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Krampus Nails done by me :)</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zlen3</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>18zlejf</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Looking for acrylic recommendations</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18zlejf/looking_for_acrylic_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>18zkus3</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Caught a bird flying around in a home that is being built but all anyone commented on are my nails 😂</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zkus3</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>18zkq5p</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>A little late but my Christmas lights nails ✨</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zkq5p</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>18zkhtf</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Did polygel on my nails for the first time. I got tired of paying for nails that I was never satisfied with. It’s actually so much fun to do it yourself:)</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tyx0i6cvdpac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>18zkf73</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Grabbed two random colors again</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kk58plhadpac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>18zk6bl</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>How to cure false nails not on hand</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18zk6bl/how_to_cure_false_nails_not_on_hand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>18zk3e8</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Nail broke 4 days before graduation manicure!</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zk3e8</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>18zk1rm</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Can I bring my own non gel polish to get Gel-X nails?</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18zk1rm/can_i_bring_my_own_non_gel_polish_to_get_gelx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>18zjkh5</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Paid 90. Opinions? [Better Photos]</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zjkh5</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>18zioms</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Help with cuticle care?</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18zioms/help_with_cuticle_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>18ziilb</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>New year, new nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7b9jf34zoac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>18zi0ov</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Progress</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zi0ov</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>18zhvrb</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>SNS Dip newbie - is this too thick?</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zhvrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>18zhv2t</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Cruelty free dupe for Essie’s Boatloads Of Love? (Ivory/Cream color)</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i20pvo47uoac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>18zhpz6</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Calling this mani “Midnight Louboutins” 🫣</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yxjhlxz4toac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>18zhq05</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>First time using a stamping plate</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqk8x1e5toac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>18zhmgv</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Sometimes you just want something plain and classic :)</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vr9aye2gsoac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>18zhhtc</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Pride Nails, Baby!</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zhhtc</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>18zh9rs</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>I think this is my favourite set I’ve done so far 🥰</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zh9rs</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>18zh54f</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Trying to get better at shaping my nails and avoiding cuticle flooding - was happy with how these came out :)</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vud8syvvooac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>18zh3wq</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>My vacay nails!</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5zjeyenooac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>18zgw1i</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Already a few days old, but I love this blue</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zgw1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>18zgknw</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Perfect nails ALWAYS 😍🩷✨</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tjhe7dqkoac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>18zbold</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Clubbed thumbs &amp; Acrylic Nails</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zbold</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>18zbmdy</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>1st set of 2024. Inspired by the other blue bow set in here</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vya32sn5knac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>18zc88j</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>i accidentally went to a chop shop</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zc88j</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>18zgekr</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>birthday nails!</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zgekr</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>18zge5x</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Who else believes that life exists on other planets?</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vhmhjuejoac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>18zdqqt</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Vetro distributor UK ?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18zdqqt/vetro_distributor_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>18zgc8y</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>New set, Gel X</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xsc80vj0joac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>18zgc64</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Loving the color! Kiss -Gel Fantasy- Letter to Ur Ex</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6fb8p30joac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>18zgb1c</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>been growing mine out</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/llqz6qwrioac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>18zg962</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Manicure with glitter French tips for $12 USD!!!!</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/it67p2udioac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>18zg7xt</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>First nails of 2024 :)</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ot23e226ioac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>18zf6kc</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>I can’t believe I let myself leave the salon like this</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zf6kc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>18zf5r9</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Square or Oval?</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zf5r9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>18zf0fa</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Something simple and sweet for the new year! 💅</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uc36aet79oac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>18zem9c</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>I really love these French acrylics</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zem9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>18zecv3</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Before throwing…</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18zecv3/before_throwing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>18zdrsy</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>This feels like a dumb question</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hw8dd25xznac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>18zdfem</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>New year nails</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0hb2c5exnac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>18zccyi</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>What would people recommend for court?</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18zccyi/what_would_people_recommend_for_court/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>18zbuqc</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Proud of my progress🥹</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gc0smpslnac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>18zbtur</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Do I have to redo there two nails, or there’s a way to fix that lifting?</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flui6r7mlnac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>18z1sce</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>from my birthday a while back!</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3l9ha2b0ykac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>18zb4n3</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>When doing French tip nails is it necessary to have the nude base colour or you can go without?</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18zb4n3/when_doing_french_tip_nails_is_it_necessary_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>18yu1gy</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Peeled and cut raw potatoes…then my nails did this?</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qg2wuzojwiac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>18yr7nv</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>How to properly use nail forms + builder gel?</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18yr7nv/how_to_properly_use_nail_forms_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>18yp287</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>What is this piece of skin that always comes up and how do I get rid of it?</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r84zukplvhac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>18zak51</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Do my nails need a break?</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18zak51/do_my_nails_need_a_break/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>18zagmm</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Nothing like a perfect ombré</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4lqt1sgbnac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>18z9ww4</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Are my nails long enough for the almond shape?</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18z9ww4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>18z91p4</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>NYE set</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdmccxuj0nac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>18z8ypr</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>help me like this new set</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4lhxw00vzmac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>18z8k9q</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>What do y’all think of this color? I hated at first but it’s growing on me. I thought it was more of a chocolate brown when I picked out lol.</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18z8k9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>18z8dzz</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>My new nails for 20€</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18z8dzz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>18z7kg7</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>14 weeks of progress with BIAB!</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1c6q0taiomac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>18z7hkb</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Thought my nails were dry when I went to sleep, woke up to blanket texture still look good though</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9a2bczvnmac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>18z7epf</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Any suggestions on what I can or should improve on?</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18z7epf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>18z7ank</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Yes or nah?</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjlqbit7mmac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>18z77gq</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Winter nails</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sao82fwflmac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>18zsc0h</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Life Pro Tip: Vasiline</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18zsc0h/life_pro_tip_vasiline/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>18zm8t4</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>🧚🏼‍♀️🦄✨ Polishes Used: Mooncat (Shade: A Midsummer’s Dream) | Mooncat (Shade: Moonfairy) | Seche Vite (Instant Gel Effect Top Coat)</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pgyn2cyqpac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>18zmsqs</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>100% Acetone still not removing polish</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18zmsqs/100_acetone_still_not_removing_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>18znidz</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Can I Repaint Over Acrylics?</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18znidz/can_i_repaint_over_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>18zs62e</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>In love with my first Death Valley Nails polish. And first thermal!</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zs62e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>18zs55y</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Putting my Christmas cabochons to use with my Doomicorn + UP + Brazilian shelf</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a0gnitvz5rac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>18zrlfu</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>OPI Nail Envy is impossible to get off</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18zrlfu/opi_nail_envy_is_impossible_to_get_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>18zr56c</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Favorite indie brands</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18zr56c/favorite_indie_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>18zqiew</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>At home mani's help plz</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18zqiew/at_home_manis_help_plz/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>18zqcmd</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Second polish already lol</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zqcmd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>18zq6li</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Best oil to soak your nails in? How long?</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18zq6li/best_oil_to_soak_your_nails_in_how_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>18zp5of</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Polish thinner for Glass Frog</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18zp5of/polish_thinner_for_glass_frog/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>18zopgo</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>My love of prugly nail polish is endless</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yz6udw40bqac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>18zomdn</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>I guess it's time to take these off!</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1pu04iaaqac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>18zobly</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>First ILNP, first Mooncat, first magnetics. You guys I’m getting nothing done this weekend.</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zobly</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>18zntni</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>what are some of your favorite duo/tri chromes?</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/28poufoo3qac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>18znshd</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Legit question... can you tell my age by my hands?</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18znshd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>18znmdi</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Do magnetics go bad/weak?</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18znmdi/do_magnetics_go_badweak/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>18zn7g2</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>So happy with the new ILNP Overcast collection (my first collection ever), just in time for some snow 🤞</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zn7g2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>18zmn6r</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Thank you!</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bgc7kv1upac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>18zm4wp</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Labeling 3.5 years of Orly Color Pass</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zm4wp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>18zlrv5</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Rite Aid fire sale, 75% off all Sally Hansen 🔥🚒</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fcsg78senpac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>18zl0xb</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>An Act of Love is the perfect winter shade</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48r0vf2yhpac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>18zkxrc</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>My first try with magnetics! Attempted the velvet trick</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dn8n38spgpac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>18zks7c</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>ILNP Tilted</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zks7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>18zki1l</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>So happy! Just got my hands on a Lemming!</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0aocu41vdpac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>18zjsum</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Glitter Ombre Almond</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zjsum</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>18zjo1a</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Getting back into stamping with the "old polish is best stamping polish" advice!</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zjo1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>18zjio9</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>The iridescence, which at first was as clear as red flame, has all but disappeared. A secret now that only flash can tell.</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zjio9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>18zjdy5</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>So I might be a little psychic?</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dtha2vl5pac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>18zj7lo</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>When talking about allergies to gel polish, what exactly IS "gel polish"?</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18zj7lo/when_talking_about_allergies_to_gel_polish_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>18zj4nk</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Summer in a bottle - KBShimmer Cruise Control</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zj4nk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>18zixo6</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>ILNP Daybreak</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdjt63s82pac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>18zini6</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>How to fix gel nails?</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18zini6/how_to_fix_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>18zidyz</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>LynB - Psychopomp</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zidyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>18zhl2x</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Mademoiselle ♡</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zhl2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>18zhflo</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Halloween manicure in January</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zhflo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>18zh9oq</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>I don’t think this was well done. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zh9oq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>18zh7vi</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>ILNP- Shockwave (H)</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zh7vi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>18zgf79</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Whatcha Aurora Borealis (Dec PPU) - Velvet hack on some nails</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/efw9usxjjoac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>18zg0uf</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Travel toothbrush holders for tool organization? Yes please! (Nail polish cabinet small update)</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zg0uf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>18zfzj1</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Mooncat Velvet Rose</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5oepc9yhgoac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>18zfaj2</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Purple pink plaid</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zfaj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>18zevhw</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Glazed pottery nails outtakes - I’ve literally never done nail art before so these are real basic lol</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zevhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>18zeuwv</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Haunted Forest dupe?</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.mooncat.com/products/haunted-forest</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>18zejgw</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Moonjelly Glow</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/machvr2q5oac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>18ze8rb</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Lord of Ringsesque</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2wkn31h3oac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>18zdzop</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>New Magnet Hack Alert</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/C1pOkJUs1Ep/?igsh=ZWMyNDBlOTQyNg==</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>18zdmso</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Soda Shoppe</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zdmso</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>18zdb34</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>My favourite colour is pink, but I don’t really do pink nails often…</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zdb34</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>18zcsi4</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>It’s so SHIFTY!!</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zcsi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>18zbk9u</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Topcoat discoloration?</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vfq4rogpjnac1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>18zbfl9</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Best base and top coat for long-lasting manicure?</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18zbfl9/best_base_and_top_coat_for_longlasting_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>18zaq7p</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>indie gel brands?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18zaq7p/indie_gel_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>18z9wtq</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Couldn't decide between a palette cleanser or a dark moody polish so I compromised with this</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18z9wtq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>18z9glw</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Nailtique Formula 2+</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18z9glw/nailtique_formula_2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>18z8zl4</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Head in the Clouds ☁️</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18z8zl4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>18z8rdj</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Rainbow connection wishlist</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7wk28pbymac1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>18z8j47</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Alchemy lacquers - lilac breasted roller 12/23 ppu</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18z8j47</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>18z85o8</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>I finally get a bouquet 💐</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18z85o8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>18z3orn</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Polishes with the most ✨iridescent / ethereal✨ vibes?</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18z3orn/polishes_with_the_most_iridescent_ethereal_vibes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>18zs6go</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>rate my polygel set</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rzs6p8ml6rac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>18zo8ah</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>The most recent set I did on myself</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zo8ah</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>18znt3i</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Mint Green and Rose Gold</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zffcayek3qac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>18zls27</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Black Matte Almonds</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bu7s86gnpac1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>18zko3b</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Marble nail art on press on tips</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zko3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>18zjbi7</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Go easy on me, im a self taught nailteach and just started doing nailart.</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2peie5t35pac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>18zesk7</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Dungeon and dragons Nail design</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18zesk7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>18zdqlu</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Vegas Nailss</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dw38w4eoznac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>18zbyeh</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>How to get a smooth finish on nailart</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9saycq5kmnac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>18z9okz</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Stamps from the past month</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18z9okz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>18z8gsu</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Glossy dark green for those cold dark winter days ❄️</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18z8gsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>18z21gh</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>A little late but some of my friends Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18z21gh</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jan  7 08:07:27 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_07.xlsx
+++ b/data/2024_01_07.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1099"/>
+  <dimension ref="A1:C1293"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19116,6 +19116,3304 @@
         </is>
       </c>
     </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>190jlbf</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Impressionist painting inspired nails by me!</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190jlbf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>190hld2</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>nail tip doesn’t fit</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/190hld2/nail_tip_doesnt_fit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>190fby9</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Does anyone know of any nail techs that aren’t home based close to Pontiac Mi or waterford Mi?</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/190fby9/does_anyone_know_of_any_nail_techs_that_arent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>190essz</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Just found this subreddit! Got something simple for a winter vibe ❄️</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/quas7wt4xwac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>190n468</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>New japanese</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190n468</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>190a52x</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Black gel polish staining nail before curing??</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/190a52x/black_gel_polish_staining_nail_before_curing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>190a3gn</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>I start my official training to become a nail tech in February!</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190a3gn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1905uy2</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Did this set on my nail biting niece and she ripped them off</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lhh2vtd0vac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1905rxc</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Is it okay to bring nail stickers into a nail salon?</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/srev47cuzuac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>190mta4</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>loving the cat eye 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l03ra2du0zac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>190mgjf</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Friendly Reminder: nails are not can openers!</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fu7o0arswyac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>190mem8</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>I’m new to getting my nails done. I got this builder gel from salon, is it good or bad?</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oohv1725wyac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>190m7p1</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>prettiest set i’ve ever had</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x53n0dv1uyac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>190ly5g</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Cheap gorgeous chrome nails !</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190ly5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>190kq8i</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Rose quartz💕</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190kq8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>190kb4b</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Current nail sitch.</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5p5ss1nayac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>190k9u8</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Need Help Fixing This Stupid Chipping</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tn7p0dgaayac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>190jlmy</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Had a Fill Today</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190jlmy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>190jk9k</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgm93rip3yac1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>190jiz7</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Structured gel with Funny bunny 🤍🐇</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/elhxmv0e3yac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>190jisr</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Finally decided to try a new salon and I think she did a great job!!</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/etntv79c3yac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>190jgwo</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>needless to say i’m obsessed with my new nail tech 🍒🍒🍒</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kf4dztxt2yac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>190je65</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Bad picture, good nails</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16un8pi22yac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>190j4cm</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>How to get these nails at home?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4alk0r9fzxac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>190iw10</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Was this set of nails worth $100??</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190iw10</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>190iv7e</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Does anyone request not putting hands in the light also..</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/190iv7e/does_anyone_request_not_putting_hands_in_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>190iula</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Accidentally, Dr. Pepper.</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ffi1m8pvwxac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>190ist6</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>birthday nails ✨</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9z89t9fwxac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>190ipsx</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Thoughts on shape/color?</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3o8pxcynvxac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>190iikv</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Are these too long??</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gy9joa6vtxac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>190i7mv</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>First time getting a matte nail 👀</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sta6gd42rxac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>190i301</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Manicure 💅</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uggqe48xpxac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>190hin9</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>My classy, nerd nails</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jw9wt0skxac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>190hcic</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer - Dustnado 🌪️</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190hcic</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>190hce5</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Hopped on the “diffused light” nail trend!</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzuu1gt7jxac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>190h9dy</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Kiss Gel Strong / Antique, a rich metallic brown I've had for probably a year but just used for the first time.</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190h9dy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>190h6n4</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>why did my nail polish crack like this after applying? can this happen when nail polish touches moisturizer?</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/190h6n4/why_did_my_nail_polish_crack_like_this_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>190h0mb</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>New year, new set!</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u89olav9gxac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>190gydy</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Nails today</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190gydy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>190gt56</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Black valentines 🖤🖤💅</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lkfwapadexac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>190gugz</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Girl dad looking for help/guidance doing nails.</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190gugz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>190gje8</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Can I just vent? Got these done while out of town. The nail tech did a beautiful job on my daughter and somehow mine ended up thick and lumpy 😔. It was $120 for both of us, and of course I tipped. Side note: I now know that almond is NOT my best shape. 😅</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190gje8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>190ggnx</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Loving the jelly + reflective combo</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190ggnx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>190gevm</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Ella + Mila After Party 😍</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qoqadtmuaxac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>190g7xu</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Top coat ruined after adding thinner help!!</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/190g7xu/top_coat_ruined_after_adding_thinner_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>190g6jn</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/np0fnfiv8xac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>190g4xp</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Do my birthday nails look ok?</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190g4xp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>190g1tw</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Classy, fem, floral</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190g1tw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>190fq9n</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Press on Nails</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/190fq9n/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>190fj61</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>January set</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190fj61</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>190fiyp</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Second time using poly gel, what do you think?</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190fiyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>190fhkm</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>First time getting acrylics in about 10 years or so..</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190fhkm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>190fgxn</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>I've got a perfect red set today!</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vv21vot2xac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>190fga8</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Which nail shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190fga8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>190fa8w</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Glazed strawberry milk try!</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190fa8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>190f0js</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Bf picked my nail color :)</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190f0js</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>190etzp</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Lavender ombré with chrome 🥰</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5h1b5gexwac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>190eg0i</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Biab/bumps and hooked nails</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190eg0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>190ef02</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>My nail art work.</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lvf25s2uwac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>190dybp</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Awh nawh I asked for a star and the nail tech drew the Star of David 😭</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvzsgipeqwac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>190dt4g</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>First timer with rubber base</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqprtcj8pwac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>190dkg4</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>still obsessed with the set💖🫶🏼🖤</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190dkg4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>190dbnd</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Abstract Sailor Moon Nails &lt;3</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190dbnd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>190d4ny</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>My normal, amazing nail tech had to cancle, she swore by this guy... I'm getting everything fixed Monday.</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190d4ny</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>190cwc7</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Nails are done for vacay &amp; I’m in 🩷</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2lw57vtwhwac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>190cvpw</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>My Own Take on the Ombré</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7q4ulwcshwac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>190cu51</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>I need help with nail shaping/filing</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r9tjbxyhhwac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>190coce</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0d8q698gwac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>190ck3a</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>I'm so happy with how these turned out</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190ck3a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>190cjqq</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Are these nails okay design/ look good?</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190cjqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>190c398</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytudnn2rbwac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>190beal</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>In love with my new set but someone told me they look like delftware</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190beal</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>190bd5i</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Strongest nail glue for press ons?</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/190bd5i/strongest_nail_glue_for_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>190bd0j</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>New nails 💅🏽</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190bd0j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>190aw99</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Obsessed with my Lisa frank mani</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190aw99</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>190ar9u</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Meow - Mood changing polish w/ a touch of cat.</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190ar9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>190anay</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Recommendation for nails which won't come off with acetone?</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/190anay/recommendation_for_nails_which_wont_come_off_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>190ada8</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Am I overreacting or are these too thick?</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190ada8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1909aju</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Cat nails!</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1909aju</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>19096wd</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Sparkle fade tips 🩵</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19096wd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1908znk</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>How much would you pay for such a manicure?</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74xaflp1ovac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1908uiy</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Latest set, I like them what do yall think</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1908uiy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1908mwm</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Kiara Sky beyond home led lamp experiences for gel manicures or other at home lamp recommendations?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1908mwm/kiara_sky_beyond_home_led_lamp_experiences_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1908kww</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>👄</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjnz52f1lvac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1907wno</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Nail growth with process pics. I’m so proud!</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1907wno</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1907r9v</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Acrylic nails design</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1907r9v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1907jl6</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>They locked the other thread but heres an update on them fixing my nails! And different color!</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fu3djxl6dvac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1907hps</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Am I jumpin' around all nimbly bimbly</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvsm3hescvac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1907ho5</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Ombré chrome</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gut2szrcvac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1906qe9</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Do I need tou use nail dehydrator and nail primer if I'll be using gel polish?</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1906qe9/do_i_need_tou_use_nail_dehydrator_and_nail_primer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1906hgq</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>My favorite go-to nail color!</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1906hgq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>19063ze</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>21M UK Based here. Cuticle / nail questions</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19063ze/21m_uk_based_here_cuticle_nail_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>190629u</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>My first hybrid ombre</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190629u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>190605g</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>My nails keep breaking no matter what I do</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rby9x1h1vac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1905oiy</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Fresh set, Prison Confessions on, and Kevin approves.</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1905oiy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1905nbm</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Decided to start learning piano for my 30th birthday. Time to say goodbye to my natural nails 🥺</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8j0tce7vyuac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1905487</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>First post here!</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68ggmcnvuuac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1904ky1</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Back to natural! I can never wear colour for long 😅</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1904ky1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1904joz</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>My Holiday set</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dzhpchhquac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>19020b0</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>love this color!</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwxip17r5uac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>190chg4</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Anyone Else's Zoya Rewards Coupons Gone?</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/190chg4/anyone_elses_zoya_rewards_coupons_gone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>190lrqk</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>My wife made it today 🥰</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190lrqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>190kv3z</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Just wanted to show my new nail space that I set up today 💗</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aayd4n5wfyac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>190k155</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Chunky Glitter Toppers</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/190k155/chunky_glitter_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>190jyxl</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>New set! 💅🏿💗✨</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akv4jzig7yac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>190js0q</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Winter themed</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190js0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>190iz0z</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>First Nailtopia Polish</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190iz0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>190if1n</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Sand Viper 🐍</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zhparqxsxac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>190ib71</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>My biggest weakness is blue holo</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gji97vxxrxac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>190i6kd</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Ghosted</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190i6kd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>190i0bx</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>My first ILNP haul!</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190i0bx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>190hn73</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Morgan Taylor Lots of Dots 🧁💕</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9icv80oxlxac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>190hjti</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>What stops you from trying new nail polish brands?</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/190hjti/what_stops_you_from_trying_new_nail_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>190h9lv</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer - Dustnado 🌪️</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190h9lv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>190gy1t</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Any ideas on how to make this more pink?</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190gy1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>190gla9</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Black Speckled Topper</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/190gla9/black_speckled_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>190fusf</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Found my grandma’s favorite nail polishes 😭🥹</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xex3eyo36xac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>190fcwo</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Sponged gradient effect</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1ngyoyv1xac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>190escb</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>It’s BOROmir not STEALmir 🌿</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190escb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>190eqkt</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Windex for nails...</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190eqkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>190e5ad</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Winter skies ❄️</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190e5ad</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>190dx1t</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Once In A Blue Moon topped with Hypnotism by Fancy Gloss</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ex1rnys3qwac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>190dte1</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>the best mani in the entire gym 😂♥️🙈 looking beautiful while i lift like a beast LOL💫</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190dte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>190douh</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Fun with thermals</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190douh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>190dnpd</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Holo beach nail art 🐚✨</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190dnpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>190djrt</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Did my nails using some cheap polish, was pleasantly surprised by the results</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s9swpdi2nwac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>190cvhi</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>A mani, a haul from Zoya sale, and a patched broken nail.</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190cvhi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>190cokt</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Mooncat -Gravity Hold Me Back</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/joveki38gwac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>190cl7v</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>I need help with nail shaping/filing</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/by6snt1lfwac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>190cfq5</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>A classic!</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190cfq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>190ccxq</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Holo Taco One Coat Black &amp; Disco Dust</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qwppfyvtdwac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>190cbyj</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Loving this film noir vibe</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190cbyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>190c75o</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Pretty and Pink</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fjd7r25lcwac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>190c5b7</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Berries 🍓🫐</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g40bmz67cwac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>190c4rj</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Finally cataloged my nail polish collection. I wanted to share my swatches with you all.</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190c4rj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>190bnth</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Neutral base with reflective glitter top coat</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qu72ciag8wac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>190bnba</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>January nails ❄️</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190bnba</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>190b0fz</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Digging in the Garden look ft Dill Weed</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190b0fz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>190azvy</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>i’m blue dabadee</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190azvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>190atph</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Was going bare trying to use a nail serum for 7 days but got impatient - no regrets 😅</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u6gjrfo32wac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>190ar3c</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Rose Jelly + All the Feelings 2.0</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mrs5jibi1wac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>190aq0t</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Loving Magnetics!</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zvgqammc1wac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>190apx5</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>That glow ✨(Mooncat what a brilliant nose)</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hw36dx351wac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1909xtq</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Crushed ice ❄️🧊</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1909xtq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1909pkv</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Swamp Gloss "It's BOROmir Not STEALomir"</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lyxynl6jtvac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1909m7s</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Cherry Red by Le Mini Macron (UUUU. Gel UV light)</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7f3azdpwsvac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1909jjg</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Winter Snowstorm ❄️</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1909jjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>190905m</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Matte Taco topcoat makes my polish pop off - ideas?</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/190905m/matte_taco_topcoat_makes_my_polish_pop_off_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1908qaj</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Mooncat Skittle</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdawnsd5mvac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1908ayv</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>🏁❤️Drag Race WERK Room🩷🏁</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1908ayv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1907ne2</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Wearing Clionadh Toxic Sludge, asking for tips for magnetics</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1907ne2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1907n7t</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Help/ recommendations</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1907n7t/help_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>19078te</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Realized something today</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19078te/realized_something_today/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>19064kc</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Phoenix Indie Paint the Town Red Stefan</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94k6y5qf2vac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>19062m4</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Like stone: El Corazon - Prisma 423/30 &amp; Confetti 520a</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19062m4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1905xa1</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>The color of moneeeeey</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1905xa1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1905n4y</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>My most beautiful jelly sandwich</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qgji7lmtyuac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1905j1c</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>How do pros handle nail fold?</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1905j1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1905b0q</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Mooncat worth it?</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1905b0q/mooncat_worth_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1904thx</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Green and sparkly for my second color this year</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1904thx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1904r9e</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Favorite thermals? This is Hard Candy by Death Valley!</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1904r9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1904gg5</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Forgotten brands of Yesteryear?</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1904gg5/forgotten_brands_of_yesteryear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1904a3k</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>New Game: Assumptions based on people’s favorite polish!</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1904a3k/new_game_assumptions_based_on_peoples_favorite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1903cpa</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>It’s giving 🧁🧁🧁</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjk3iv80huac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1903cdq</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Seriously in love ♥️</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1903cdq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1902qeo</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Asked for polygel, got this instead 🙃</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1902qeo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1902c8l</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>nail is starting to break, what can i do?</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08josf2m8uac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1902a1t</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>ILNP Hex</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1902a1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>19028zj</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Lumen Glass Jellyfish</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r3cdl57u7uac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1901z3o</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Cuticle oil Recs</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1901z3o/cuticle_oil_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1901tm7</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Shooting Star by ILNP - the perfect magnetic nailpolish ❤️</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1901tm7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1901nge</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Mooncat Full Scream Ahead</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1901nge</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1901iwh</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Winter ❄️🩵</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1901iwh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>19017vl</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>{PR} So much sparkles! 🤩</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25opbdavytac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1900qmq</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Feeling very proud of restoring this 2017 indie</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1900qmq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1900btc</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>I couldnt decide between these two options now im not sure if i like my hands this different from each other.</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/98fhilwrqtac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>190047u</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>What is your favorite nail polish? You can only choose one.</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/190047u/what_is_your_favorite_nail_polish_you_can_only/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>18zy47i</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Trying out combos</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/314aci9p2tac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>190mq9g</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>What technique/s can I use to achieve this “agate” effect</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thshi2mxzyac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>190kewq</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Some winter nails I’ve done recently.</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190kewq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>190js0t</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>My eldest (they/he) requested nonbinary nails</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfh2sqfo5yac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>190hwug</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>A month early, for Lunar New Year</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190hwug</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>190feak</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>baby blue my melody press ons~! ʚ♡ɞ</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190feak</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>190eoeu</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Oil slick set for my friend :)</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z12ii9s5wwac1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>190efvn</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>My nail art work.</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gpjq4w9uwac1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>190edj7</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190edj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>190dgbp</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>First attempt at squiggle art!</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190dgbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>190c52y</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Dip &amp; gel</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190c52y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>190aq09</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Tried out some new gold stickers!</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/190aq09</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>190ajn4</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Full set (beginner) </t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/08j8gu000wac1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1908qdc</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Male Mani!</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1908qdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1905thq</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>nye nails</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1905thq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1905jmx</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>I tried 🤷🏼‍♀️</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1905jmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>19034ir</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Candy themed nails by me!</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19034ir</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>